<commit_message>
reference input sheet is open at first page
</commit_message>
<xml_diff>
--- a/PMConverter/administration/Project data input sheet.xlsx
+++ b/PMConverter/administration/Project data input sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-37320" yWindow="-5595" windowWidth="36180" windowHeight="16440" tabRatio="772" activeTab="10"/>
+    <workbookView xWindow="-37320" yWindow="-5595" windowWidth="36180" windowHeight="16440" tabRatio="772"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline Schedule" sheetId="1" r:id="rId1"/>
@@ -1735,6 +1735,18 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1746,18 +1758,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="75">
@@ -2254,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CT61"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -2279,30 +2279,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:98" ht="15" customHeight="1">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50" t="s">
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50" t="s">
+      <c r="J1" s="54"/>
+      <c r="K1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:98" ht="21">
       <c r="A2" s="2" t="s">
@@ -2360,8 +2360,8 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -2382,8 +2382,8 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -2407,10 +2407,10 @@
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="51">
         <v>38824.333333333299</v>
       </c>
-      <c r="G5" s="56"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
@@ -2521,10 +2521,10 @@
       <c r="E6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="55">
+      <c r="F6" s="51">
         <v>38908.333333333299</v>
       </c>
-      <c r="G6" s="56"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="4" t="s">
         <v>35</v>
       </c>
@@ -2631,10 +2631,10 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="55">
+      <c r="F7" s="51">
         <v>38824.333333333299</v>
       </c>
-      <c r="G7" s="56"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="4" t="s">
         <v>35</v>
       </c>
@@ -2741,10 +2741,10 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="55">
+      <c r="F8" s="51">
         <v>38824.333333333299</v>
       </c>
-      <c r="G8" s="56"/>
+      <c r="G8" s="52"/>
       <c r="H8" s="4" t="s">
         <v>28</v>
       </c>
@@ -2855,10 +2855,10 @@
       <c r="E9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="51">
         <v>38936.333333333299</v>
       </c>
-      <c r="G9" s="56"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2967,10 +2967,10 @@
       <c r="E10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="51">
         <v>39020.333333333299</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="4" t="s">
         <v>54</v>
       </c>
@@ -3079,8 +3079,8 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3182,10 +3182,10 @@
       <c r="E12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="51">
         <v>39062.333333333299</v>
       </c>
-      <c r="G12" s="56"/>
+      <c r="G12" s="52"/>
       <c r="H12" s="4" t="s">
         <v>64</v>
       </c>
@@ -3293,10 +3293,10 @@
       <c r="E13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="51">
         <v>39062.333333333299</v>
       </c>
-      <c r="G13" s="56"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="4" t="s">
         <v>70</v>
       </c>
@@ -3404,10 +3404,10 @@
       <c r="E14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="51">
         <v>39080.333333333299</v>
       </c>
-      <c r="G14" s="56"/>
+      <c r="G14" s="52"/>
       <c r="H14" s="4" t="s">
         <v>76</v>
       </c>
@@ -3515,10 +3515,10 @@
       <c r="E15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15" s="51">
         <v>39080.333333333299</v>
       </c>
-      <c r="G15" s="56"/>
+      <c r="G15" s="52"/>
       <c r="H15" s="4" t="s">
         <v>83</v>
       </c>
@@ -3626,10 +3626,10 @@
       <c r="E16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="51">
         <v>39094.333333333299</v>
       </c>
-      <c r="G16" s="56"/>
+      <c r="G16" s="52"/>
       <c r="H16" s="4" t="s">
         <v>88</v>
       </c>
@@ -3733,8 +3733,8 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -3834,10 +3834,10 @@
       <c r="E18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="55">
+      <c r="F18" s="51">
         <v>39115.333333333299</v>
       </c>
-      <c r="G18" s="56"/>
+      <c r="G18" s="52"/>
       <c r="H18" s="4" t="s">
         <v>35</v>
       </c>
@@ -3945,10 +3945,10 @@
       <c r="E19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="55">
+      <c r="F19" s="51">
         <v>39143.333333333299</v>
       </c>
-      <c r="G19" s="56"/>
+      <c r="G19" s="52"/>
       <c r="H19" s="4" t="s">
         <v>83</v>
       </c>
@@ -4056,10 +4056,10 @@
       <c r="E20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20" s="51">
         <v>39157.333333333299</v>
       </c>
-      <c r="G20" s="56"/>
+      <c r="G20" s="52"/>
       <c r="H20" s="4" t="s">
         <v>108</v>
       </c>
@@ -4167,10 +4167,10 @@
       <c r="E21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="55">
+      <c r="F21" s="51">
         <v>39178.333333333299</v>
       </c>
-      <c r="G21" s="56"/>
+      <c r="G21" s="52"/>
       <c r="H21" s="4" t="s">
         <v>108</v>
       </c>
@@ -4274,8 +4274,8 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -4375,10 +4375,10 @@
       <c r="E23" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="55">
+      <c r="F23" s="51">
         <v>39199.333333333299</v>
       </c>
-      <c r="G23" s="56"/>
+      <c r="G23" s="52"/>
       <c r="H23" s="4" t="s">
         <v>35</v>
       </c>
@@ -4486,10 +4486,10 @@
       <c r="E24" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F24" s="55">
+      <c r="F24" s="51">
         <v>39227.333333333299</v>
       </c>
-      <c r="G24" s="56"/>
+      <c r="G24" s="52"/>
       <c r="H24" s="4" t="s">
         <v>83</v>
       </c>
@@ -4595,10 +4595,10 @@
         <v>120</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="55">
+      <c r="F25" s="51">
         <v>39199.333333333299</v>
       </c>
-      <c r="G25" s="56"/>
+      <c r="G25" s="52"/>
       <c r="H25" s="4" t="s">
         <v>83</v>
       </c>
@@ -4702,8 +4702,8 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -4803,10 +4803,10 @@
       <c r="E27" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F27" s="55">
+      <c r="F27" s="51">
         <v>39241.333333333299</v>
       </c>
-      <c r="G27" s="56"/>
+      <c r="G27" s="52"/>
       <c r="H27" s="4" t="s">
         <v>83</v>
       </c>
@@ -4914,10 +4914,10 @@
       <c r="E28" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F28" s="55">
+      <c r="F28" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G28" s="56"/>
+      <c r="G28" s="52"/>
       <c r="H28" s="4" t="s">
         <v>83</v>
       </c>
@@ -5023,10 +5023,10 @@
         <v>144</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="55">
+      <c r="F29" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G29" s="56"/>
+      <c r="G29" s="52"/>
       <c r="H29" s="4" t="s">
         <v>83</v>
       </c>
@@ -5134,10 +5134,10 @@
       <c r="E30" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="55">
+      <c r="F30" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G30" s="56"/>
+      <c r="G30" s="52"/>
       <c r="H30" s="4" t="s">
         <v>35</v>
       </c>
@@ -5245,10 +5245,10 @@
       <c r="E31" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F31" s="55">
+      <c r="F31" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G31" s="56"/>
+      <c r="G31" s="52"/>
       <c r="H31" s="4" t="s">
         <v>76</v>
       </c>
@@ -5356,10 +5356,10 @@
       <c r="E32" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="55">
+      <c r="F32" s="51">
         <v>39358.416666666701</v>
       </c>
-      <c r="G32" s="56"/>
+      <c r="G32" s="52"/>
       <c r="H32" s="4" t="s">
         <v>35</v>
       </c>
@@ -5463,8 +5463,8 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -5562,10 +5562,10 @@
       <c r="E34" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F34" s="55">
+      <c r="F34" s="51">
         <v>39309.416666666701</v>
       </c>
-      <c r="G34" s="56"/>
+      <c r="G34" s="52"/>
       <c r="H34" s="4" t="s">
         <v>83</v>
       </c>
@@ -5667,8 +5667,8 @@
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -5766,10 +5766,10 @@
         <v>144</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="55">
+      <c r="F36" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G36" s="56"/>
+      <c r="G36" s="52"/>
       <c r="H36" s="4" t="s">
         <v>83</v>
       </c>
@@ -5875,10 +5875,10 @@
         <v>144</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="55">
+      <c r="F37" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G37" s="56"/>
+      <c r="G37" s="52"/>
       <c r="H37" s="4" t="s">
         <v>83</v>
       </c>
@@ -5986,10 +5986,10 @@
       <c r="E38" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F38" s="55">
+      <c r="F38" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G38" s="56"/>
+      <c r="G38" s="52"/>
       <c r="H38" s="4" t="s">
         <v>108</v>
       </c>
@@ -6095,10 +6095,10 @@
         <v>144</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="55">
+      <c r="F39" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G39" s="56"/>
+      <c r="G39" s="52"/>
       <c r="H39" s="4" t="s">
         <v>35</v>
       </c>
@@ -6204,10 +6204,10 @@
         <v>144</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="55">
+      <c r="F40" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G40" s="56"/>
+      <c r="G40" s="52"/>
       <c r="H40" s="4" t="s">
         <v>76</v>
       </c>
@@ -6315,10 +6315,10 @@
       <c r="E41" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F41" s="55">
+      <c r="F41" s="51">
         <v>39344.416666666701</v>
       </c>
-      <c r="G41" s="56"/>
+      <c r="G41" s="52"/>
       <c r="H41" s="4" t="s">
         <v>198</v>
       </c>
@@ -6424,10 +6424,10 @@
       <c r="E42" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="F42" s="55">
+      <c r="F42" s="51">
         <v>39351.416666666701</v>
       </c>
-      <c r="G42" s="56"/>
+      <c r="G42" s="52"/>
       <c r="H42" s="4" t="s">
         <v>35</v>
       </c>
@@ -6531,8 +6531,8 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
@@ -6630,10 +6630,10 @@
         <v>210</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="55">
+      <c r="F44" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G44" s="56"/>
+      <c r="G44" s="52"/>
       <c r="H44" s="4" t="s">
         <v>83</v>
       </c>
@@ -6739,10 +6739,10 @@
         <v>210</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="55">
+      <c r="F45" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G45" s="56"/>
+      <c r="G45" s="52"/>
       <c r="H45" s="4" t="s">
         <v>83</v>
       </c>
@@ -6850,10 +6850,10 @@
       <c r="E46" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="F46" s="55">
+      <c r="F46" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G46" s="56"/>
+      <c r="G46" s="52"/>
       <c r="H46" s="4" t="s">
         <v>108</v>
       </c>
@@ -6959,10 +6959,10 @@
         <v>210</v>
       </c>
       <c r="E47" s="4"/>
-      <c r="F47" s="55">
+      <c r="F47" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G47" s="56"/>
+      <c r="G47" s="52"/>
       <c r="H47" s="4" t="s">
         <v>35</v>
       </c>
@@ -7068,10 +7068,10 @@
         <v>210</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="F48" s="55">
+      <c r="F48" s="51">
         <v>39323.416666666701</v>
       </c>
-      <c r="G48" s="56"/>
+      <c r="G48" s="52"/>
       <c r="H48" s="4" t="s">
         <v>76</v>
       </c>
@@ -7179,10 +7179,10 @@
       <c r="E49" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="F49" s="55">
+      <c r="F49" s="51">
         <v>39344.416666666701</v>
       </c>
-      <c r="G49" s="56"/>
+      <c r="G49" s="52"/>
       <c r="H49" s="4" t="s">
         <v>198</v>
       </c>
@@ -7288,10 +7288,10 @@
       <c r="E50" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="F50" s="55">
+      <c r="F50" s="51">
         <v>39351.416666666701</v>
       </c>
-      <c r="G50" s="56"/>
+      <c r="G50" s="52"/>
       <c r="H50" s="4" t="s">
         <v>35</v>
       </c>
@@ -7395,8 +7395,8 @@
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -7496,10 +7496,10 @@
       <c r="E52" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F52" s="55">
+      <c r="F52" s="51">
         <v>39351.416666666701</v>
       </c>
-      <c r="G52" s="56"/>
+      <c r="G52" s="52"/>
       <c r="H52" s="4" t="s">
         <v>108</v>
       </c>
@@ -7605,10 +7605,10 @@
         <v>245</v>
       </c>
       <c r="E53" s="4"/>
-      <c r="F53" s="55">
+      <c r="F53" s="51">
         <v>39379.416666666701</v>
       </c>
-      <c r="G53" s="56"/>
+      <c r="G53" s="52"/>
       <c r="H53" s="4" t="s">
         <v>76</v>
       </c>
@@ -7698,7 +7698,7 @@
       <c r="CS53" s="41"/>
       <c r="CT53" s="42"/>
     </row>
-    <row r="54" spans="1:98">
+    <row r="54" spans="1:98" ht="21">
       <c r="A54" s="10" t="s">
         <v>246</v>
       </c>
@@ -7712,10 +7712,10 @@
         <v>249</v>
       </c>
       <c r="E54" s="4"/>
-      <c r="F54" s="55">
+      <c r="F54" s="51">
         <v>39386.416666666701</v>
       </c>
-      <c r="G54" s="56"/>
+      <c r="G54" s="52"/>
       <c r="H54" s="4" t="s">
         <v>108</v>
       </c>
@@ -7805,7 +7805,7 @@
       <c r="CS54" s="41"/>
       <c r="CT54" s="42"/>
     </row>
-    <row r="55" spans="1:98">
+    <row r="55" spans="1:98" ht="21">
       <c r="A55" s="10" t="s">
         <v>250</v>
       </c>
@@ -7821,10 +7821,10 @@
       <c r="E55" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F55" s="55">
+      <c r="F55" s="51">
         <v>39386.416666666701</v>
       </c>
-      <c r="G55" s="56"/>
+      <c r="G55" s="52"/>
       <c r="H55" s="4" t="s">
         <v>108</v>
       </c>
@@ -7928,10 +7928,10 @@
         <v>257</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="F56" s="55">
+      <c r="F56" s="51">
         <v>39407.416666666701</v>
       </c>
-      <c r="G56" s="56"/>
+      <c r="G56" s="52"/>
       <c r="H56" s="4" t="s">
         <v>83</v>
       </c>
@@ -8035,10 +8035,10 @@
         <v>257</v>
       </c>
       <c r="E57" s="4"/>
-      <c r="F57" s="55">
+      <c r="F57" s="51">
         <v>39407.416666666701</v>
       </c>
-      <c r="G57" s="56"/>
+      <c r="G57" s="52"/>
       <c r="H57" s="4" t="s">
         <v>83</v>
       </c>
@@ -8142,10 +8142,10 @@
         <v>257</v>
       </c>
       <c r="E58" s="4"/>
-      <c r="F58" s="55">
+      <c r="F58" s="51">
         <v>39407.416666666701</v>
       </c>
-      <c r="G58" s="56"/>
+      <c r="G58" s="52"/>
       <c r="H58" s="4" t="s">
         <v>198</v>
       </c>
@@ -8251,10 +8251,10 @@
       <c r="E59" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="F59" s="55">
+      <c r="F59" s="51">
         <v>39407.416666666701</v>
       </c>
-      <c r="G59" s="56"/>
+      <c r="G59" s="52"/>
       <c r="H59" s="4" t="s">
         <v>198</v>
       </c>
@@ -8360,10 +8360,10 @@
       <c r="E60" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="F60" s="55">
+      <c r="F60" s="51">
         <v>39414.416666666701</v>
       </c>
-      <c r="G60" s="56"/>
+      <c r="G60" s="52"/>
       <c r="H60" s="4" t="s">
         <v>108</v>
       </c>
@@ -8469,10 +8469,10 @@
         <v>277</v>
       </c>
       <c r="E61" s="4"/>
-      <c r="F61" s="55">
+      <c r="F61" s="51">
         <v>39435.416666666701</v>
       </c>
-      <c r="G61" s="56"/>
+      <c r="G61" s="52"/>
       <c r="H61" s="4" t="s">
         <v>198</v>
       </c>
@@ -8625,40 +8625,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -8820,7 +8820,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="14">
         <v>75</v>
       </c>
@@ -8858,7 +8858,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="14">
         <v>210000</v>
       </c>
@@ -8896,7 +8896,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="14">
         <v>3765.3101000000001</v>
       </c>
@@ -8934,7 +8934,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57"/>
+      <c r="R10" s="53"/>
       <c r="S10" s="14">
         <v>1876.54</v>
       </c>
@@ -8972,7 +8972,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="14">
         <v>0.01</v>
       </c>
@@ -9010,7 +9010,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57"/>
+      <c r="R12" s="53"/>
       <c r="S12" s="14">
         <v>67701.789099999995</v>
       </c>
@@ -9078,7 +9078,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57"/>
+      <c r="R14" s="53"/>
       <c r="S14" s="14">
         <v>29084.800800000001</v>
       </c>
@@ -9116,7 +9116,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57"/>
+      <c r="R15" s="53"/>
       <c r="S15" s="14">
         <v>5701.7602999999999</v>
       </c>
@@ -9154,7 +9154,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57"/>
+      <c r="R16" s="53"/>
       <c r="S16" s="14">
         <v>118883.4062</v>
       </c>
@@ -9192,7 +9192,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57"/>
+      <c r="R17" s="53"/>
       <c r="S17" s="14">
         <v>12330.0098</v>
       </c>
@@ -9230,7 +9230,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57"/>
+      <c r="R18" s="53"/>
       <c r="S18" s="14">
         <v>236361.8438</v>
       </c>
@@ -9298,7 +9298,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57"/>
+      <c r="R20" s="53"/>
       <c r="S20" s="14">
         <v>137501.3125</v>
       </c>
@@ -9336,7 +9336,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57"/>
+      <c r="R21" s="53"/>
       <c r="S21" s="14">
         <v>123579.32030000001</v>
       </c>
@@ -9374,7 +9374,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57"/>
+      <c r="R22" s="53"/>
       <c r="S22" s="14">
         <v>132874.10939999999</v>
       </c>
@@ -9412,7 +9412,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57"/>
+      <c r="R23" s="53"/>
       <c r="S23" s="14">
         <v>129748.9219</v>
       </c>
@@ -9480,7 +9480,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57"/>
+      <c r="R25" s="53"/>
       <c r="S25" s="14">
         <v>351653.1875</v>
       </c>
@@ -9518,7 +9518,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="14">
         <v>234654.5938</v>
       </c>
@@ -9556,7 +9556,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57"/>
+      <c r="R27" s="53"/>
       <c r="S27" s="14">
         <v>85523.570300000007</v>
       </c>
@@ -9624,7 +9624,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57"/>
+      <c r="R29" s="53"/>
       <c r="S29" s="14">
         <v>142112</v>
       </c>
@@ -9662,7 +9662,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57"/>
+      <c r="R30" s="53"/>
       <c r="S30" s="14">
         <v>7673</v>
       </c>
@@ -9700,7 +9700,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57"/>
+      <c r="R31" s="53"/>
       <c r="S31" s="14">
         <v>37704.960899999998</v>
       </c>
@@ -9738,7 +9738,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57"/>
+      <c r="R32" s="53"/>
       <c r="S32" s="14">
         <v>18563</v>
       </c>
@@ -9776,7 +9776,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57"/>
+      <c r="R33" s="53"/>
       <c r="S33" s="14">
         <v>3840</v>
       </c>
@@ -9814,7 +9814,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57"/>
+      <c r="R34" s="53"/>
       <c r="S34" s="14">
         <v>81649.601599999995</v>
       </c>
@@ -9882,7 +9882,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="14">
         <v>0.01</v>
       </c>
@@ -9950,7 +9950,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57"/>
+      <c r="R38" s="53"/>
       <c r="S38" s="14">
         <v>7673</v>
       </c>
@@ -9988,7 +9988,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57"/>
+      <c r="R39" s="53"/>
       <c r="S39" s="14">
         <v>37704.960899999998</v>
       </c>
@@ -10026,7 +10026,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57"/>
+      <c r="R40" s="53"/>
       <c r="S40" s="14">
         <v>106140</v>
       </c>
@@ -10064,7 +10064,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57"/>
+      <c r="R41" s="53"/>
       <c r="S41" s="14">
         <v>25475</v>
       </c>
@@ -10102,7 +10102,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57"/>
+      <c r="R42" s="53"/>
       <c r="S42" s="14">
         <v>6400</v>
       </c>
@@ -10140,7 +10140,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57"/>
+      <c r="R43" s="53"/>
       <c r="S43" s="14">
         <v>0.01</v>
       </c>
@@ -10178,7 +10178,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57"/>
+      <c r="R44" s="53"/>
       <c r="S44" s="14">
         <v>79149.601599999995</v>
       </c>
@@ -10246,7 +10246,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57"/>
+      <c r="R46" s="53"/>
       <c r="S46" s="14">
         <v>7673</v>
       </c>
@@ -10284,7 +10284,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57"/>
+      <c r="R47" s="53"/>
       <c r="S47" s="14">
         <v>34452.960899999998</v>
       </c>
@@ -10322,7 +10322,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57"/>
+      <c r="R48" s="53"/>
       <c r="S48" s="14">
         <v>46116</v>
       </c>
@@ -10360,7 +10360,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57"/>
+      <c r="R49" s="53"/>
       <c r="S49" s="14">
         <v>16771</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57"/>
+      <c r="R50" s="53"/>
       <c r="S50" s="14">
         <v>5120</v>
       </c>
@@ -10436,7 +10436,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57"/>
+      <c r="R51" s="53"/>
       <c r="S51" s="14">
         <v>0.01</v>
       </c>
@@ -10474,7 +10474,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57"/>
+      <c r="R52" s="53"/>
       <c r="S52" s="14">
         <v>38149.601600000002</v>
       </c>
@@ -10542,7 +10542,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57"/>
+      <c r="R54" s="53"/>
       <c r="S54" s="14">
         <v>23538.800800000001</v>
       </c>
@@ -10580,7 +10580,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57"/>
+      <c r="R55" s="53"/>
       <c r="S55" s="14">
         <v>48000</v>
       </c>
@@ -10618,7 +10618,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57"/>
+      <c r="R56" s="53"/>
       <c r="S56" s="14">
         <v>87000</v>
       </c>
@@ -10656,7 +10656,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57"/>
+      <c r="R57" s="53"/>
       <c r="S57" s="14">
         <v>2156.0601000000001</v>
       </c>
@@ -10694,7 +10694,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57"/>
+      <c r="R58" s="53"/>
       <c r="S58" s="14">
         <v>33000</v>
       </c>
@@ -10732,7 +10732,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57"/>
+      <c r="R59" s="53"/>
       <c r="S59" s="14">
         <v>16000</v>
       </c>
@@ -10770,7 +10770,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57"/>
+      <c r="R60" s="53"/>
       <c r="S60" s="14">
         <v>38817.851600000002</v>
       </c>
@@ -10808,7 +10808,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57"/>
+      <c r="R61" s="53"/>
       <c r="S61" s="14">
         <v>32000</v>
       </c>
@@ -10846,7 +10846,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57"/>
+      <c r="R62" s="53"/>
       <c r="S62" s="14">
         <v>99800</v>
       </c>
@@ -10884,7 +10884,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57"/>
+      <c r="R63" s="53"/>
       <c r="S63" s="14">
         <v>138400</v>
       </c>
@@ -10918,7 +10918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -10933,15 +10933,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.1" customHeight="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="24"/>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="E1" s="53"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="24"/>
       <c r="G1" s="25" t="s">
         <v>331</v>
@@ -11689,20 +11689,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50" t="s">
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50" t="s">
+      <c r="F1" s="54"/>
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="50"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="21">
       <c r="A2" s="2" t="s">
@@ -12026,19 +12026,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50"/>
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54"/>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="54" t="s">
         <v>302</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" ht="21">
       <c r="A2" s="2" t="s">
@@ -13279,40 +13279,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -13474,7 +13474,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57">
+      <c r="R7" s="53">
         <v>0</v>
       </c>
       <c r="S7" s="14">
@@ -13512,7 +13512,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57">
+      <c r="R8" s="53">
         <v>0</v>
       </c>
       <c r="S8" s="14">
@@ -13552,7 +13552,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57">
+      <c r="R9" s="53">
         <v>0</v>
       </c>
       <c r="S9" s="14">
@@ -13592,7 +13592,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57">
+      <c r="R10" s="53">
         <v>0</v>
       </c>
       <c r="S10" s="14">
@@ -13630,7 +13630,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57">
+      <c r="R11" s="53">
         <v>0</v>
       </c>
       <c r="S11" s="14">
@@ -13668,7 +13668,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57">
+      <c r="R12" s="53">
         <v>0</v>
       </c>
       <c r="S12" s="14">
@@ -13736,7 +13736,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57">
+      <c r="R14" s="53">
         <v>0</v>
       </c>
       <c r="S14" s="14">
@@ -13774,7 +13774,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57">
+      <c r="R15" s="53">
         <v>0</v>
       </c>
       <c r="S15" s="14">
@@ -13812,7 +13812,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57">
+      <c r="R16" s="53">
         <v>0</v>
       </c>
       <c r="S16" s="14">
@@ -13850,7 +13850,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57">
+      <c r="R17" s="53">
         <v>0</v>
       </c>
       <c r="S17" s="14">
@@ -13888,7 +13888,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57">
+      <c r="R18" s="53">
         <v>0</v>
       </c>
       <c r="S18" s="14">
@@ -13956,7 +13956,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57">
+      <c r="R20" s="53">
         <v>0</v>
       </c>
       <c r="S20" s="14">
@@ -13994,7 +13994,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57">
+      <c r="R21" s="53">
         <v>0</v>
       </c>
       <c r="S21" s="14">
@@ -14032,7 +14032,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57">
+      <c r="R22" s="53">
         <v>0</v>
       </c>
       <c r="S22" s="14">
@@ -14070,7 +14070,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57">
+      <c r="R23" s="53">
         <v>0</v>
       </c>
       <c r="S23" s="14">
@@ -14138,7 +14138,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57">
+      <c r="R25" s="53">
         <v>0</v>
       </c>
       <c r="S25" s="14">
@@ -14176,7 +14176,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57">
+      <c r="R26" s="53">
         <v>0</v>
       </c>
       <c r="S26" s="14">
@@ -14214,7 +14214,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57">
+      <c r="R27" s="53">
         <v>0</v>
       </c>
       <c r="S27" s="14">
@@ -14282,7 +14282,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57">
+      <c r="R29" s="53">
         <v>0</v>
       </c>
       <c r="S29" s="14">
@@ -14320,7 +14320,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57">
+      <c r="R30" s="53">
         <v>0</v>
       </c>
       <c r="S30" s="14">
@@ -14358,7 +14358,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57">
+      <c r="R31" s="53">
         <v>0</v>
       </c>
       <c r="S31" s="14">
@@ -14396,7 +14396,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57">
+      <c r="R32" s="53">
         <v>0</v>
       </c>
       <c r="S32" s="14">
@@ -14434,7 +14434,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57">
+      <c r="R33" s="53">
         <v>0</v>
       </c>
       <c r="S33" s="14">
@@ -14472,7 +14472,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57">
+      <c r="R34" s="53">
         <v>0</v>
       </c>
       <c r="S34" s="14">
@@ -14540,7 +14540,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57">
+      <c r="R36" s="53">
         <v>0</v>
       </c>
       <c r="S36" s="14">
@@ -14608,7 +14608,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57">
+      <c r="R38" s="53">
         <v>0</v>
       </c>
       <c r="S38" s="14">
@@ -14646,7 +14646,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57">
+      <c r="R39" s="53">
         <v>0</v>
       </c>
       <c r="S39" s="14">
@@ -14684,7 +14684,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57">
+      <c r="R40" s="53">
         <v>0</v>
       </c>
       <c r="S40" s="14">
@@ -14722,7 +14722,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57">
+      <c r="R41" s="53">
         <v>0</v>
       </c>
       <c r="S41" s="14">
@@ -14760,7 +14760,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57">
+      <c r="R42" s="53">
         <v>0</v>
       </c>
       <c r="S42" s="14">
@@ -14798,7 +14798,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57">
+      <c r="R43" s="53">
         <v>0</v>
       </c>
       <c r="S43" s="14">
@@ -14836,7 +14836,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57">
+      <c r="R44" s="53">
         <v>0</v>
       </c>
       <c r="S44" s="14">
@@ -14904,7 +14904,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57">
+      <c r="R46" s="53">
         <v>0</v>
       </c>
       <c r="S46" s="14">
@@ -14942,7 +14942,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57">
+      <c r="R47" s="53">
         <v>0</v>
       </c>
       <c r="S47" s="14">
@@ -14980,7 +14980,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57">
+      <c r="R48" s="53">
         <v>0</v>
       </c>
       <c r="S48" s="14">
@@ -15018,7 +15018,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57">
+      <c r="R49" s="53">
         <v>0</v>
       </c>
       <c r="S49" s="14">
@@ -15056,7 +15056,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57">
+      <c r="R50" s="53">
         <v>0</v>
       </c>
       <c r="S50" s="14">
@@ -15094,7 +15094,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57">
+      <c r="R51" s="53">
         <v>0</v>
       </c>
       <c r="S51" s="14">
@@ -15132,7 +15132,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57">
+      <c r="R52" s="53">
         <v>0</v>
       </c>
       <c r="S52" s="14">
@@ -15200,7 +15200,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57">
+      <c r="R54" s="53">
         <v>0</v>
       </c>
       <c r="S54" s="14">
@@ -15238,7 +15238,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57">
+      <c r="R55" s="53">
         <v>0</v>
       </c>
       <c r="S55" s="14">
@@ -15276,7 +15276,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57">
+      <c r="R56" s="53">
         <v>0</v>
       </c>
       <c r="S56" s="14">
@@ -15314,7 +15314,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57">
+      <c r="R57" s="53">
         <v>0</v>
       </c>
       <c r="S57" s="14">
@@ -15352,7 +15352,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57">
+      <c r="R58" s="53">
         <v>0</v>
       </c>
       <c r="S58" s="14">
@@ -15390,7 +15390,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57">
+      <c r="R59" s="53">
         <v>0</v>
       </c>
       <c r="S59" s="14">
@@ -15428,7 +15428,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57">
+      <c r="R60" s="53">
         <v>0</v>
       </c>
       <c r="S60" s="14">
@@ -15466,7 +15466,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57">
+      <c r="R61" s="53">
         <v>0</v>
       </c>
       <c r="S61" s="14">
@@ -15504,7 +15504,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57">
+      <c r="R62" s="53">
         <v>0</v>
       </c>
       <c r="S62" s="14">
@@ -15542,7 +15542,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57">
+      <c r="R63" s="53">
         <v>0</v>
       </c>
       <c r="S63" s="14">
@@ -15617,40 +15617,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -15812,7 +15812,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57">
+      <c r="R7" s="53">
         <v>0</v>
       </c>
       <c r="S7" s="14">
@@ -15852,7 +15852,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57">
+      <c r="R8" s="53">
         <v>0</v>
       </c>
       <c r="S8" s="14">
@@ -15892,7 +15892,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57">
+      <c r="R9" s="53">
         <v>0</v>
       </c>
       <c r="S9" s="14">
@@ -15932,7 +15932,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57">
+      <c r="R10" s="53">
         <v>0</v>
       </c>
       <c r="S10" s="14">
@@ -15972,7 +15972,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57">
+      <c r="R11" s="53">
         <v>0</v>
       </c>
       <c r="S11" s="14">
@@ -16012,7 +16012,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57">
+      <c r="R12" s="53">
         <v>0</v>
       </c>
       <c r="S12" s="14">
@@ -16080,7 +16080,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57">
+      <c r="R14" s="53">
         <v>0</v>
       </c>
       <c r="S14" s="14">
@@ -16118,7 +16118,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57">
+      <c r="R15" s="53">
         <v>0</v>
       </c>
       <c r="S15" s="14">
@@ -16156,7 +16156,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57">
+      <c r="R16" s="53">
         <v>0</v>
       </c>
       <c r="S16" s="14">
@@ -16194,7 +16194,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57">
+      <c r="R17" s="53">
         <v>0</v>
       </c>
       <c r="S17" s="14">
@@ -16232,7 +16232,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57">
+      <c r="R18" s="53">
         <v>0</v>
       </c>
       <c r="S18" s="14">
@@ -16300,7 +16300,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57">
+      <c r="R20" s="53">
         <v>0</v>
       </c>
       <c r="S20" s="14">
@@ -16338,7 +16338,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57">
+      <c r="R21" s="53">
         <v>0</v>
       </c>
       <c r="S21" s="14">
@@ -16376,7 +16376,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57">
+      <c r="R22" s="53">
         <v>0</v>
       </c>
       <c r="S22" s="14">
@@ -16414,7 +16414,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57">
+      <c r="R23" s="53">
         <v>0</v>
       </c>
       <c r="S23" s="14">
@@ -16482,7 +16482,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57">
+      <c r="R25" s="53">
         <v>0</v>
       </c>
       <c r="S25" s="14">
@@ -16520,7 +16520,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57">
+      <c r="R26" s="53">
         <v>0</v>
       </c>
       <c r="S26" s="14">
@@ -16558,7 +16558,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57">
+      <c r="R27" s="53">
         <v>0</v>
       </c>
       <c r="S27" s="14">
@@ -16626,7 +16626,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57">
+      <c r="R29" s="53">
         <v>0</v>
       </c>
       <c r="S29" s="14">
@@ -16664,7 +16664,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57">
+      <c r="R30" s="53">
         <v>0</v>
       </c>
       <c r="S30" s="14">
@@ -16702,7 +16702,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57">
+      <c r="R31" s="53">
         <v>0</v>
       </c>
       <c r="S31" s="14">
@@ -16740,7 +16740,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57">
+      <c r="R32" s="53">
         <v>0</v>
       </c>
       <c r="S32" s="14">
@@ -16778,7 +16778,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57">
+      <c r="R33" s="53">
         <v>0</v>
       </c>
       <c r="S33" s="14">
@@ -16816,7 +16816,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57">
+      <c r="R34" s="53">
         <v>0</v>
       </c>
       <c r="S34" s="14">
@@ -16884,7 +16884,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57">
+      <c r="R36" s="53">
         <v>0</v>
       </c>
       <c r="S36" s="14">
@@ -16952,7 +16952,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57">
+      <c r="R38" s="53">
         <v>0</v>
       </c>
       <c r="S38" s="14">
@@ -16990,7 +16990,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57">
+      <c r="R39" s="53">
         <v>0</v>
       </c>
       <c r="S39" s="14">
@@ -17028,7 +17028,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57">
+      <c r="R40" s="53">
         <v>0</v>
       </c>
       <c r="S40" s="14">
@@ -17066,7 +17066,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57">
+      <c r="R41" s="53">
         <v>0</v>
       </c>
       <c r="S41" s="14">
@@ -17104,7 +17104,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57">
+      <c r="R42" s="53">
         <v>0</v>
       </c>
       <c r="S42" s="14">
@@ -17142,7 +17142,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57">
+      <c r="R43" s="53">
         <v>0</v>
       </c>
       <c r="S43" s="14">
@@ -17180,7 +17180,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57">
+      <c r="R44" s="53">
         <v>0</v>
       </c>
       <c r="S44" s="14">
@@ -17248,7 +17248,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57">
+      <c r="R46" s="53">
         <v>0</v>
       </c>
       <c r="S46" s="14">
@@ -17286,7 +17286,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57">
+      <c r="R47" s="53">
         <v>0</v>
       </c>
       <c r="S47" s="14">
@@ -17324,7 +17324,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57">
+      <c r="R48" s="53">
         <v>0</v>
       </c>
       <c r="S48" s="14">
@@ -17362,7 +17362,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57">
+      <c r="R49" s="53">
         <v>0</v>
       </c>
       <c r="S49" s="14">
@@ -17400,7 +17400,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57">
+      <c r="R50" s="53">
         <v>0</v>
       </c>
       <c r="S50" s="14">
@@ -17438,7 +17438,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57">
+      <c r="R51" s="53">
         <v>0</v>
       </c>
       <c r="S51" s="14">
@@ -17476,7 +17476,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57">
+      <c r="R52" s="53">
         <v>0</v>
       </c>
       <c r="S52" s="14">
@@ -17544,7 +17544,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57">
+      <c r="R54" s="53">
         <v>0</v>
       </c>
       <c r="S54" s="14">
@@ -17582,7 +17582,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57">
+      <c r="R55" s="53">
         <v>0</v>
       </c>
       <c r="S55" s="14">
@@ -17620,7 +17620,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57">
+      <c r="R56" s="53">
         <v>0</v>
       </c>
       <c r="S56" s="14">
@@ -17658,7 +17658,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57">
+      <c r="R57" s="53">
         <v>0</v>
       </c>
       <c r="S57" s="14">
@@ -17696,7 +17696,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57">
+      <c r="R58" s="53">
         <v>0</v>
       </c>
       <c r="S58" s="14">
@@ -17734,7 +17734,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57">
+      <c r="R59" s="53">
         <v>0</v>
       </c>
       <c r="S59" s="14">
@@ -17772,7 +17772,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57">
+      <c r="R60" s="53">
         <v>0</v>
       </c>
       <c r="S60" s="14">
@@ -17810,7 +17810,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57">
+      <c r="R61" s="53">
         <v>0</v>
       </c>
       <c r="S61" s="14">
@@ -17848,7 +17848,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57">
+      <c r="R62" s="53">
         <v>0</v>
       </c>
       <c r="S62" s="14">
@@ -17886,7 +17886,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57">
+      <c r="R63" s="53">
         <v>0</v>
       </c>
       <c r="S63" s="14">
@@ -17961,40 +17961,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -18156,7 +18156,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="14">
         <v>75</v>
       </c>
@@ -18194,7 +18194,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="14">
         <v>210000</v>
       </c>
@@ -18232,7 +18232,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="14">
         <v>3765.3101000000001</v>
       </c>
@@ -18270,7 +18270,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57"/>
+      <c r="R10" s="53"/>
       <c r="S10" s="14">
         <v>1876.54</v>
       </c>
@@ -18308,7 +18308,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="14">
         <v>0.01</v>
       </c>
@@ -18346,7 +18346,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57"/>
+      <c r="R12" s="53"/>
       <c r="S12" s="14">
         <v>67701.789099999995</v>
       </c>
@@ -18414,7 +18414,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57"/>
+      <c r="R14" s="53"/>
       <c r="S14" s="14">
         <v>29084.800800000001</v>
       </c>
@@ -18452,7 +18452,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57"/>
+      <c r="R15" s="53"/>
       <c r="S15" s="14">
         <v>5701.7602999999999</v>
       </c>
@@ -18490,7 +18490,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57"/>
+      <c r="R16" s="53"/>
       <c r="S16" s="14">
         <v>110554.45</v>
       </c>
@@ -18528,7 +18528,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57"/>
+      <c r="R17" s="53"/>
       <c r="S17" s="14">
         <v>12330.0098</v>
       </c>
@@ -18566,7 +18566,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57"/>
+      <c r="R18" s="53"/>
       <c r="S18" s="14">
         <v>236361.8438</v>
       </c>
@@ -18632,7 +18632,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57"/>
+      <c r="R20" s="53"/>
       <c r="S20" s="14">
         <v>0</v>
       </c>
@@ -18668,7 +18668,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57"/>
+      <c r="R21" s="53"/>
       <c r="S21" s="14">
         <v>0</v>
       </c>
@@ -18704,7 +18704,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57"/>
+      <c r="R22" s="53"/>
       <c r="S22" s="14">
         <v>0</v>
       </c>
@@ -18740,7 +18740,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57"/>
+      <c r="R23" s="53"/>
       <c r="S23" s="14">
         <v>0</v>
       </c>
@@ -18806,7 +18806,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57"/>
+      <c r="R25" s="53"/>
       <c r="S25" s="14">
         <v>0</v>
       </c>
@@ -18842,7 +18842,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="14">
         <v>0</v>
       </c>
@@ -18878,7 +18878,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57"/>
+      <c r="R27" s="53"/>
       <c r="S27" s="14">
         <v>0</v>
       </c>
@@ -18944,7 +18944,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57"/>
+      <c r="R29" s="53"/>
       <c r="S29" s="14">
         <v>0</v>
       </c>
@@ -18980,7 +18980,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57"/>
+      <c r="R30" s="53"/>
       <c r="S30" s="14">
         <v>0</v>
       </c>
@@ -19016,7 +19016,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57"/>
+      <c r="R31" s="53"/>
       <c r="S31" s="14">
         <v>0</v>
       </c>
@@ -19052,7 +19052,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57"/>
+      <c r="R32" s="53"/>
       <c r="S32" s="14">
         <v>0</v>
       </c>
@@ -19088,7 +19088,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57"/>
+      <c r="R33" s="53"/>
       <c r="S33" s="14">
         <v>0</v>
       </c>
@@ -19124,7 +19124,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57"/>
+      <c r="R34" s="53"/>
       <c r="S34" s="14">
         <v>0</v>
       </c>
@@ -19190,7 +19190,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="14">
         <v>0</v>
       </c>
@@ -19256,7 +19256,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57"/>
+      <c r="R38" s="53"/>
       <c r="S38" s="14">
         <v>0</v>
       </c>
@@ -19292,7 +19292,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57"/>
+      <c r="R39" s="53"/>
       <c r="S39" s="14">
         <v>0</v>
       </c>
@@ -19328,7 +19328,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57"/>
+      <c r="R40" s="53"/>
       <c r="S40" s="14">
         <v>0</v>
       </c>
@@ -19364,7 +19364,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57"/>
+      <c r="R41" s="53"/>
       <c r="S41" s="14">
         <v>0</v>
       </c>
@@ -19400,7 +19400,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57"/>
+      <c r="R42" s="53"/>
       <c r="S42" s="14">
         <v>0</v>
       </c>
@@ -19436,7 +19436,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57"/>
+      <c r="R43" s="53"/>
       <c r="S43" s="14">
         <v>0</v>
       </c>
@@ -19472,7 +19472,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57"/>
+      <c r="R44" s="53"/>
       <c r="S44" s="14">
         <v>0</v>
       </c>
@@ -19538,7 +19538,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57"/>
+      <c r="R46" s="53"/>
       <c r="S46" s="14">
         <v>0</v>
       </c>
@@ -19574,7 +19574,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57"/>
+      <c r="R47" s="53"/>
       <c r="S47" s="14">
         <v>0</v>
       </c>
@@ -19610,7 +19610,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57"/>
+      <c r="R48" s="53"/>
       <c r="S48" s="14">
         <v>0</v>
       </c>
@@ -19646,7 +19646,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57"/>
+      <c r="R49" s="53"/>
       <c r="S49" s="14">
         <v>0</v>
       </c>
@@ -19682,7 +19682,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57"/>
+      <c r="R50" s="53"/>
       <c r="S50" s="14">
         <v>0</v>
       </c>
@@ -19718,7 +19718,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57"/>
+      <c r="R51" s="53"/>
       <c r="S51" s="14">
         <v>0</v>
       </c>
@@ -19754,7 +19754,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57"/>
+      <c r="R52" s="53"/>
       <c r="S52" s="14">
         <v>0</v>
       </c>
@@ -19820,7 +19820,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57"/>
+      <c r="R54" s="53"/>
       <c r="S54" s="14">
         <v>0</v>
       </c>
@@ -19856,7 +19856,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57"/>
+      <c r="R55" s="53"/>
       <c r="S55" s="14">
         <v>0</v>
       </c>
@@ -19892,7 +19892,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57"/>
+      <c r="R56" s="53"/>
       <c r="S56" s="14">
         <v>0</v>
       </c>
@@ -19928,7 +19928,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57"/>
+      <c r="R57" s="53"/>
       <c r="S57" s="14">
         <v>0</v>
       </c>
@@ -19964,7 +19964,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57"/>
+      <c r="R58" s="53"/>
       <c r="S58" s="14">
         <v>0</v>
       </c>
@@ -20000,7 +20000,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57"/>
+      <c r="R59" s="53"/>
       <c r="S59" s="14">
         <v>0</v>
       </c>
@@ -20036,7 +20036,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57"/>
+      <c r="R60" s="53"/>
       <c r="S60" s="14">
         <v>0</v>
       </c>
@@ -20072,7 +20072,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57"/>
+      <c r="R61" s="53"/>
       <c r="S61" s="14">
         <v>0</v>
       </c>
@@ -20108,7 +20108,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57"/>
+      <c r="R62" s="53"/>
       <c r="S62" s="14">
         <v>0</v>
       </c>
@@ -20144,7 +20144,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57"/>
+      <c r="R63" s="53"/>
       <c r="S63" s="14">
         <v>0</v>
       </c>
@@ -20217,40 +20217,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -20412,7 +20412,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="14">
         <v>75</v>
       </c>
@@ -20450,7 +20450,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="14">
         <v>210000</v>
       </c>
@@ -20488,7 +20488,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="14">
         <v>3765.3101000000001</v>
       </c>
@@ -20526,7 +20526,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57"/>
+      <c r="R10" s="53"/>
       <c r="S10" s="14">
         <v>1876.54</v>
       </c>
@@ -20564,7 +20564,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="14">
         <v>0.01</v>
       </c>
@@ -20602,7 +20602,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57"/>
+      <c r="R12" s="53"/>
       <c r="S12" s="14">
         <v>67701.789099999995</v>
       </c>
@@ -20670,7 +20670,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57"/>
+      <c r="R14" s="53"/>
       <c r="S14" s="14">
         <v>29084.800800000001</v>
       </c>
@@ -20708,7 +20708,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57"/>
+      <c r="R15" s="53"/>
       <c r="S15" s="14">
         <v>5701.7602999999999</v>
       </c>
@@ -20746,7 +20746,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57"/>
+      <c r="R16" s="53"/>
       <c r="S16" s="14">
         <v>118883.4062</v>
       </c>
@@ -20784,7 +20784,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57"/>
+      <c r="R17" s="53"/>
       <c r="S17" s="14">
         <v>12330.0098</v>
       </c>
@@ -20822,7 +20822,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57"/>
+      <c r="R18" s="53"/>
       <c r="S18" s="14">
         <v>236361.8438</v>
       </c>
@@ -20890,7 +20890,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57"/>
+      <c r="R20" s="53"/>
       <c r="S20" s="14">
         <v>137501.3125</v>
       </c>
@@ -20928,7 +20928,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57"/>
+      <c r="R21" s="53"/>
       <c r="S21" s="14">
         <v>123579.32030000001</v>
       </c>
@@ -20966,7 +20966,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57"/>
+      <c r="R22" s="53"/>
       <c r="S22" s="14">
         <v>132874.10939999999</v>
       </c>
@@ -21004,7 +21004,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57"/>
+      <c r="R23" s="53"/>
       <c r="S23" s="14">
         <v>129748.9219</v>
       </c>
@@ -21070,7 +21070,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57"/>
+      <c r="R25" s="53"/>
       <c r="S25" s="14">
         <v>0</v>
       </c>
@@ -21106,7 +21106,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="14">
         <v>0</v>
       </c>
@@ -21142,7 +21142,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57"/>
+      <c r="R27" s="53"/>
       <c r="S27" s="14">
         <v>0</v>
       </c>
@@ -21208,7 +21208,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57"/>
+      <c r="R29" s="53"/>
       <c r="S29" s="14">
         <v>0</v>
       </c>
@@ -21244,7 +21244,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57"/>
+      <c r="R30" s="53"/>
       <c r="S30" s="14">
         <v>0</v>
       </c>
@@ -21280,7 +21280,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57"/>
+      <c r="R31" s="53"/>
       <c r="S31" s="14">
         <v>0</v>
       </c>
@@ -21316,7 +21316,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57"/>
+      <c r="R32" s="53"/>
       <c r="S32" s="14">
         <v>0</v>
       </c>
@@ -21352,7 +21352,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57"/>
+      <c r="R33" s="53"/>
       <c r="S33" s="14">
         <v>0</v>
       </c>
@@ -21388,7 +21388,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57"/>
+      <c r="R34" s="53"/>
       <c r="S34" s="14">
         <v>0</v>
       </c>
@@ -21454,7 +21454,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="14">
         <v>0</v>
       </c>
@@ -21520,7 +21520,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57"/>
+      <c r="R38" s="53"/>
       <c r="S38" s="14">
         <v>0</v>
       </c>
@@ -21556,7 +21556,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57"/>
+      <c r="R39" s="53"/>
       <c r="S39" s="14">
         <v>0</v>
       </c>
@@ -21592,7 +21592,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57"/>
+      <c r="R40" s="53"/>
       <c r="S40" s="14">
         <v>0</v>
       </c>
@@ -21628,7 +21628,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57"/>
+      <c r="R41" s="53"/>
       <c r="S41" s="14">
         <v>0</v>
       </c>
@@ -21664,7 +21664,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57"/>
+      <c r="R42" s="53"/>
       <c r="S42" s="14">
         <v>0</v>
       </c>
@@ -21700,7 +21700,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57"/>
+      <c r="R43" s="53"/>
       <c r="S43" s="14">
         <v>0</v>
       </c>
@@ -21736,7 +21736,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57"/>
+      <c r="R44" s="53"/>
       <c r="S44" s="14">
         <v>0</v>
       </c>
@@ -21802,7 +21802,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57"/>
+      <c r="R46" s="53"/>
       <c r="S46" s="14">
         <v>0</v>
       </c>
@@ -21838,7 +21838,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57"/>
+      <c r="R47" s="53"/>
       <c r="S47" s="14">
         <v>0</v>
       </c>
@@ -21874,7 +21874,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57"/>
+      <c r="R48" s="53"/>
       <c r="S48" s="14">
         <v>0</v>
       </c>
@@ -21910,7 +21910,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57"/>
+      <c r="R49" s="53"/>
       <c r="S49" s="14">
         <v>0</v>
       </c>
@@ -21946,7 +21946,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57"/>
+      <c r="R50" s="53"/>
       <c r="S50" s="14">
         <v>0</v>
       </c>
@@ -21982,7 +21982,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57"/>
+      <c r="R51" s="53"/>
       <c r="S51" s="14">
         <v>0</v>
       </c>
@@ -22018,7 +22018,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57"/>
+      <c r="R52" s="53"/>
       <c r="S52" s="14">
         <v>0</v>
       </c>
@@ -22084,7 +22084,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57"/>
+      <c r="R54" s="53"/>
       <c r="S54" s="14">
         <v>0</v>
       </c>
@@ -22120,7 +22120,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57"/>
+      <c r="R55" s="53"/>
       <c r="S55" s="14">
         <v>0</v>
       </c>
@@ -22156,7 +22156,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57"/>
+      <c r="R56" s="53"/>
       <c r="S56" s="14">
         <v>0</v>
       </c>
@@ -22192,7 +22192,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57"/>
+      <c r="R57" s="53"/>
       <c r="S57" s="14">
         <v>0</v>
       </c>
@@ -22228,7 +22228,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57"/>
+      <c r="R58" s="53"/>
       <c r="S58" s="14">
         <v>0</v>
       </c>
@@ -22264,7 +22264,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57"/>
+      <c r="R59" s="53"/>
       <c r="S59" s="14">
         <v>0</v>
       </c>
@@ -22300,7 +22300,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57"/>
+      <c r="R60" s="53"/>
       <c r="S60" s="14">
         <v>0</v>
       </c>
@@ -22336,7 +22336,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57"/>
+      <c r="R61" s="53"/>
       <c r="S61" s="14">
         <v>0</v>
       </c>
@@ -22372,7 +22372,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57"/>
+      <c r="R62" s="53"/>
       <c r="S62" s="14">
         <v>0</v>
       </c>
@@ -22408,7 +22408,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57"/>
+      <c r="R63" s="53"/>
       <c r="S63" s="14">
         <v>0</v>
       </c>
@@ -22481,40 +22481,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -22676,7 +22676,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="14">
         <v>75</v>
       </c>
@@ -22714,7 +22714,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="14">
         <v>210000</v>
       </c>
@@ -22752,7 +22752,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="14">
         <v>3765.3101000000001</v>
       </c>
@@ -22790,7 +22790,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57"/>
+      <c r="R10" s="53"/>
       <c r="S10" s="14">
         <v>1876.54</v>
       </c>
@@ -22828,7 +22828,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="14">
         <v>0.01</v>
       </c>
@@ -22866,7 +22866,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57"/>
+      <c r="R12" s="53"/>
       <c r="S12" s="14">
         <v>67701.789099999995</v>
       </c>
@@ -22934,7 +22934,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57"/>
+      <c r="R14" s="53"/>
       <c r="S14" s="14">
         <v>29084.800800000001</v>
       </c>
@@ -22972,7 +22972,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57"/>
+      <c r="R15" s="53"/>
       <c r="S15" s="14">
         <v>5701.7602999999999</v>
       </c>
@@ -23010,7 +23010,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57"/>
+      <c r="R16" s="53"/>
       <c r="S16" s="14">
         <v>118883.4062</v>
       </c>
@@ -23048,7 +23048,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57"/>
+      <c r="R17" s="53"/>
       <c r="S17" s="14">
         <v>12330.0098</v>
       </c>
@@ -23086,7 +23086,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57"/>
+      <c r="R18" s="53"/>
       <c r="S18" s="14">
         <v>236361.8438</v>
       </c>
@@ -23154,7 +23154,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57"/>
+      <c r="R20" s="53"/>
       <c r="S20" s="14">
         <v>137501.3125</v>
       </c>
@@ -23192,7 +23192,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57"/>
+      <c r="R21" s="53"/>
       <c r="S21" s="14">
         <v>123579.32030000001</v>
       </c>
@@ -23230,7 +23230,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57"/>
+      <c r="R22" s="53"/>
       <c r="S22" s="14">
         <v>132874.10939999999</v>
       </c>
@@ -23268,7 +23268,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57"/>
+      <c r="R23" s="53"/>
       <c r="S23" s="14">
         <v>129748.9219</v>
       </c>
@@ -23336,7 +23336,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57"/>
+      <c r="R25" s="53"/>
       <c r="S25" s="14">
         <v>351653.1875</v>
       </c>
@@ -23372,7 +23372,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="14">
         <v>0</v>
       </c>
@@ -23410,7 +23410,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57"/>
+      <c r="R27" s="53"/>
       <c r="S27" s="14">
         <v>85523.570300000007</v>
       </c>
@@ -23476,7 +23476,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57"/>
+      <c r="R29" s="53"/>
       <c r="S29" s="14">
         <v>0</v>
       </c>
@@ -23512,7 +23512,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57"/>
+      <c r="R30" s="53"/>
       <c r="S30" s="14">
         <v>0</v>
       </c>
@@ -23548,7 +23548,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57"/>
+      <c r="R31" s="53"/>
       <c r="S31" s="14">
         <v>0</v>
       </c>
@@ -23584,7 +23584,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57"/>
+      <c r="R32" s="53"/>
       <c r="S32" s="14">
         <v>0</v>
       </c>
@@ -23620,7 +23620,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57"/>
+      <c r="R33" s="53"/>
       <c r="S33" s="14">
         <v>0</v>
       </c>
@@ -23656,7 +23656,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57"/>
+      <c r="R34" s="53"/>
       <c r="S34" s="14">
         <v>0</v>
       </c>
@@ -23722,7 +23722,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="14">
         <v>0</v>
       </c>
@@ -23788,7 +23788,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57"/>
+      <c r="R38" s="53"/>
       <c r="S38" s="14">
         <v>0</v>
       </c>
@@ -23824,7 +23824,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57"/>
+      <c r="R39" s="53"/>
       <c r="S39" s="14">
         <v>0</v>
       </c>
@@ -23860,7 +23860,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57"/>
+      <c r="R40" s="53"/>
       <c r="S40" s="14">
         <v>0</v>
       </c>
@@ -23896,7 +23896,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57"/>
+      <c r="R41" s="53"/>
       <c r="S41" s="14">
         <v>0</v>
       </c>
@@ -23932,7 +23932,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57"/>
+      <c r="R42" s="53"/>
       <c r="S42" s="14">
         <v>0</v>
       </c>
@@ -23968,7 +23968,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57"/>
+      <c r="R43" s="53"/>
       <c r="S43" s="14">
         <v>0</v>
       </c>
@@ -24004,7 +24004,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57"/>
+      <c r="R44" s="53"/>
       <c r="S44" s="14">
         <v>0</v>
       </c>
@@ -24070,7 +24070,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57"/>
+      <c r="R46" s="53"/>
       <c r="S46" s="14">
         <v>0</v>
       </c>
@@ -24106,7 +24106,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57"/>
+      <c r="R47" s="53"/>
       <c r="S47" s="14">
         <v>0</v>
       </c>
@@ -24142,7 +24142,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57"/>
+      <c r="R48" s="53"/>
       <c r="S48" s="14">
         <v>0</v>
       </c>
@@ -24178,7 +24178,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57"/>
+      <c r="R49" s="53"/>
       <c r="S49" s="14">
         <v>0</v>
       </c>
@@ -24214,7 +24214,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57"/>
+      <c r="R50" s="53"/>
       <c r="S50" s="14">
         <v>0</v>
       </c>
@@ -24250,7 +24250,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57"/>
+      <c r="R51" s="53"/>
       <c r="S51" s="14">
         <v>0</v>
       </c>
@@ -24286,7 +24286,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57"/>
+      <c r="R52" s="53"/>
       <c r="S52" s="14">
         <v>0</v>
       </c>
@@ -24352,7 +24352,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57"/>
+      <c r="R54" s="53"/>
       <c r="S54" s="14">
         <v>0</v>
       </c>
@@ -24388,7 +24388,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57"/>
+      <c r="R55" s="53"/>
       <c r="S55" s="14">
         <v>0</v>
       </c>
@@ -24424,7 +24424,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57"/>
+      <c r="R56" s="53"/>
       <c r="S56" s="14">
         <v>0</v>
       </c>
@@ -24460,7 +24460,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57"/>
+      <c r="R57" s="53"/>
       <c r="S57" s="14">
         <v>0</v>
       </c>
@@ -24496,7 +24496,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57"/>
+      <c r="R58" s="53"/>
       <c r="S58" s="14">
         <v>0</v>
       </c>
@@ -24532,7 +24532,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57"/>
+      <c r="R59" s="53"/>
       <c r="S59" s="14">
         <v>0</v>
       </c>
@@ -24568,7 +24568,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57"/>
+      <c r="R60" s="53"/>
       <c r="S60" s="14">
         <v>0</v>
       </c>
@@ -24604,7 +24604,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57"/>
+      <c r="R61" s="53"/>
       <c r="S61" s="14">
         <v>0</v>
       </c>
@@ -24640,7 +24640,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57"/>
+      <c r="R62" s="53"/>
       <c r="S62" s="14">
         <v>0</v>
       </c>
@@ -24676,7 +24676,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57"/>
+      <c r="R63" s="53"/>
       <c r="S63" s="14">
         <v>0</v>
       </c>
@@ -24749,40 +24749,40 @@
       <c r="G1" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50" t="s">
+      <c r="A3" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="21.95" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -24944,7 +24944,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="57"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="14">
         <v>75</v>
       </c>
@@ -24982,7 +24982,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="57"/>
+      <c r="R8" s="53"/>
       <c r="S8" s="14">
         <v>210000</v>
       </c>
@@ -25020,7 +25020,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="57"/>
+      <c r="R9" s="53"/>
       <c r="S9" s="14">
         <v>3765.3101000000001</v>
       </c>
@@ -25058,7 +25058,7 @@
       <c r="O10" s="13"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="57"/>
+      <c r="R10" s="53"/>
       <c r="S10" s="14">
         <v>1876.54</v>
       </c>
@@ -25096,7 +25096,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="57"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="14">
         <v>0.01</v>
       </c>
@@ -25134,7 +25134,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="57"/>
+      <c r="R12" s="53"/>
       <c r="S12" s="14">
         <v>67701.789099999995</v>
       </c>
@@ -25202,7 +25202,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="57"/>
+      <c r="R14" s="53"/>
       <c r="S14" s="14">
         <v>29084.800800000001</v>
       </c>
@@ -25240,7 +25240,7 @@
       <c r="O15" s="13"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="57"/>
+      <c r="R15" s="53"/>
       <c r="S15" s="14">
         <v>5701.7602999999999</v>
       </c>
@@ -25278,7 +25278,7 @@
       <c r="O16" s="13"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="57"/>
+      <c r="R16" s="53"/>
       <c r="S16" s="14">
         <v>118883.4062</v>
       </c>
@@ -25316,7 +25316,7 @@
       <c r="O17" s="13"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="57"/>
+      <c r="R17" s="53"/>
       <c r="S17" s="14">
         <v>12330.0098</v>
       </c>
@@ -25354,7 +25354,7 @@
       <c r="O18" s="13"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="57"/>
+      <c r="R18" s="53"/>
       <c r="S18" s="14">
         <v>236361.8438</v>
       </c>
@@ -25422,7 +25422,7 @@
       <c r="O20" s="13"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="57"/>
+      <c r="R20" s="53"/>
       <c r="S20" s="14">
         <v>137501.3125</v>
       </c>
@@ -25460,7 +25460,7 @@
       <c r="O21" s="13"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="57"/>
+      <c r="R21" s="53"/>
       <c r="S21" s="14">
         <v>123579.32030000001</v>
       </c>
@@ -25498,7 +25498,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="57"/>
+      <c r="R22" s="53"/>
       <c r="S22" s="14">
         <v>132874.10939999999</v>
       </c>
@@ -25536,7 +25536,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="57"/>
+      <c r="R23" s="53"/>
       <c r="S23" s="14">
         <v>129748.9219</v>
       </c>
@@ -25604,7 +25604,7 @@
       <c r="O25" s="13"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="57"/>
+      <c r="R25" s="53"/>
       <c r="S25" s="14">
         <v>351653.1875</v>
       </c>
@@ -25642,7 +25642,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="57"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="14">
         <v>226446.59</v>
       </c>
@@ -25680,7 +25680,7 @@
       <c r="O27" s="13"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="13"/>
-      <c r="R27" s="57"/>
+      <c r="R27" s="53"/>
       <c r="S27" s="14">
         <v>85523.570300000007</v>
       </c>
@@ -25748,7 +25748,7 @@
       <c r="O29" s="13"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="57"/>
+      <c r="R29" s="53"/>
       <c r="S29" s="14">
         <v>142112</v>
       </c>
@@ -25786,7 +25786,7 @@
       <c r="O30" s="13"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="13"/>
-      <c r="R30" s="57"/>
+      <c r="R30" s="53"/>
       <c r="S30" s="14">
         <v>7673</v>
       </c>
@@ -25824,7 +25824,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="57"/>
+      <c r="R31" s="53"/>
       <c r="S31" s="14">
         <v>37704.960899999998</v>
       </c>
@@ -25862,7 +25862,7 @@
       <c r="O32" s="13"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="13"/>
-      <c r="R32" s="57"/>
+      <c r="R32" s="53"/>
       <c r="S32" s="14">
         <v>18563</v>
       </c>
@@ -25900,7 +25900,7 @@
       <c r="O33" s="13"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="57"/>
+      <c r="R33" s="53"/>
       <c r="S33" s="14">
         <v>3840</v>
       </c>
@@ -25938,7 +25938,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="57"/>
+      <c r="R34" s="53"/>
       <c r="S34" s="14">
         <v>81649.601599999995</v>
       </c>
@@ -26006,7 +26006,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="17"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="57"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="14">
         <v>0.01</v>
       </c>
@@ -26074,7 +26074,7 @@
       <c r="O38" s="13"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="57"/>
+      <c r="R38" s="53"/>
       <c r="S38" s="14">
         <v>7673</v>
       </c>
@@ -26112,7 +26112,7 @@
       <c r="O39" s="13"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="57"/>
+      <c r="R39" s="53"/>
       <c r="S39" s="14">
         <v>37704.960899999998</v>
       </c>
@@ -26150,7 +26150,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="57"/>
+      <c r="R40" s="53"/>
       <c r="S40" s="14">
         <v>106140</v>
       </c>
@@ -26188,7 +26188,7 @@
       <c r="O41" s="13"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="57"/>
+      <c r="R41" s="53"/>
       <c r="S41" s="14">
         <v>25475</v>
       </c>
@@ -26226,7 +26226,7 @@
       <c r="O42" s="13"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="57"/>
+      <c r="R42" s="53"/>
       <c r="S42" s="14">
         <v>6400</v>
       </c>
@@ -26264,7 +26264,7 @@
       <c r="O43" s="13"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="57"/>
+      <c r="R43" s="53"/>
       <c r="S43" s="14">
         <v>0.01</v>
       </c>
@@ -26302,7 +26302,7 @@
       <c r="O44" s="13"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="13"/>
-      <c r="R44" s="57"/>
+      <c r="R44" s="53"/>
       <c r="S44" s="14">
         <v>77487.199999999997</v>
       </c>
@@ -26370,7 +26370,7 @@
       <c r="O46" s="13"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="57"/>
+      <c r="R46" s="53"/>
       <c r="S46" s="14">
         <v>7673</v>
       </c>
@@ -26408,7 +26408,7 @@
       <c r="O47" s="13"/>
       <c r="P47" s="17"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="57"/>
+      <c r="R47" s="53"/>
       <c r="S47" s="14">
         <v>34452.960899999998</v>
       </c>
@@ -26446,7 +26446,7 @@
       <c r="O48" s="13"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="57"/>
+      <c r="R48" s="53"/>
       <c r="S48" s="14">
         <v>46116</v>
       </c>
@@ -26484,7 +26484,7 @@
       <c r="O49" s="13"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="57"/>
+      <c r="R49" s="53"/>
       <c r="S49" s="14">
         <v>16771</v>
       </c>
@@ -26522,7 +26522,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="17"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="57"/>
+      <c r="R50" s="53"/>
       <c r="S50" s="14">
         <v>5120</v>
       </c>
@@ -26560,7 +26560,7 @@
       <c r="O51" s="13"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="57"/>
+      <c r="R51" s="53"/>
       <c r="S51" s="14">
         <v>0.01</v>
       </c>
@@ -26598,7 +26598,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="57"/>
+      <c r="R52" s="53"/>
       <c r="S52" s="14">
         <v>38149.601600000002</v>
       </c>
@@ -26664,7 +26664,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="57"/>
+      <c r="R54" s="53"/>
       <c r="S54" s="14">
         <v>0</v>
       </c>
@@ -26700,7 +26700,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="13"/>
-      <c r="R55" s="57"/>
+      <c r="R55" s="53"/>
       <c r="S55" s="14">
         <v>0</v>
       </c>
@@ -26736,7 +26736,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="17"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="57"/>
+      <c r="R56" s="53"/>
       <c r="S56" s="14">
         <v>0</v>
       </c>
@@ -26772,7 +26772,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="17"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="57"/>
+      <c r="R57" s="53"/>
       <c r="S57" s="14">
         <v>0</v>
       </c>
@@ -26808,7 +26808,7 @@
       <c r="O58" s="13"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="13"/>
-      <c r="R58" s="57"/>
+      <c r="R58" s="53"/>
       <c r="S58" s="14">
         <v>0</v>
       </c>
@@ -26844,7 +26844,7 @@
       <c r="O59" s="13"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="13"/>
-      <c r="R59" s="57"/>
+      <c r="R59" s="53"/>
       <c r="S59" s="14">
         <v>0</v>
       </c>
@@ -26880,7 +26880,7 @@
       <c r="O60" s="13"/>
       <c r="P60" s="17"/>
       <c r="Q60" s="13"/>
-      <c r="R60" s="57"/>
+      <c r="R60" s="53"/>
       <c r="S60" s="14">
         <v>0</v>
       </c>
@@ -26916,7 +26916,7 @@
       <c r="O61" s="13"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="13"/>
-      <c r="R61" s="57"/>
+      <c r="R61" s="53"/>
       <c r="S61" s="14">
         <v>0</v>
       </c>
@@ -26952,7 +26952,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="13"/>
-      <c r="R62" s="57"/>
+      <c r="R62" s="53"/>
       <c r="S62" s="14">
         <v>0</v>
       </c>
@@ -26988,7 +26988,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="17"/>
       <c r="Q63" s="13"/>
-      <c r="R63" s="57"/>
+      <c r="R63" s="53"/>
       <c r="S63" s="14">
         <v>0</v>
       </c>

</xml_diff>